<commit_message>
update website, update readme
</commit_message>
<xml_diff>
--- a/processing/processed_data_codebook.xlsx
+++ b/processing/processed_data_codebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/CDS-Data/08_Projects/temprisk/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB983DF-A61E-414F-87E1-2DFE42E8764D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36495CDB-A802-F044-B8EC-FA10F61D17E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20660" activeTab="2" xr2:uid="{98993F0A-1EA3-D645-AB10-C27C59724E4A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{98993F0A-1EA3-D645-AB10-C27C59724E4A}"/>
   </bookViews>
   <sheets>
     <sheet name=" intercor_data.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="214">
   <si>
     <t>panel</t>
   </si>
@@ -174,15 +174,6 @@
     <t>meas_pair_lbl</t>
   </si>
   <si>
-    <t>name_pair_lbl</t>
-  </si>
-  <si>
-    <t>name_a_lbl</t>
-  </si>
-  <si>
-    <t>name_b_lbl</t>
-  </si>
-  <si>
     <t>n_mean</t>
   </si>
   <si>
@@ -402,9 +393,6 @@
     <t>Skewness of variable B responses</t>
   </si>
   <si>
-    <t>Age group of respondents</t>
-  </si>
-  <si>
     <t>Measure category of variable A (pro, fre, beh)</t>
   </si>
   <si>
@@ -657,30 +645,9 @@
     <t xml:space="preserve">Correlation between sampling errors of effect sizes being aggregated </t>
   </si>
   <si>
-    <t>Label for measure A (category-domain)</t>
-  </si>
-  <si>
-    <t>Label for measure B (category-domain)</t>
-  </si>
-  <si>
     <t>Measure category pair label (e.g., propensity-frequency)</t>
   </si>
   <si>
-    <t>Measure category-domain pair label (e.g., Propensity-General-Frequency-Smoking)</t>
-  </si>
-  <si>
-    <t>Measure category of measure A (e.g., pro)</t>
-  </si>
-  <si>
-    <t>Domain name of measure A  (e.g., gen)</t>
-  </si>
-  <si>
-    <t>Measure category of measure B (e.g., pro)</t>
-  </si>
-  <si>
-    <t>Domain name of measure B  (e.g., gen)</t>
-  </si>
-  <si>
     <t>Mean age of the respondents (i.e., mean of the mean age of respondents )</t>
   </si>
   <si>
@@ -694,6 +661,15 @@
   </si>
   <si>
     <t>Whether variable B is a domain general or specific measure</t>
+  </si>
+  <si>
+    <t>domain_pair_lbl</t>
+  </si>
+  <si>
+    <t>Measure category-domain pair label (e.g., Propensity-General_Frequency-Smoking)</t>
+  </si>
+  <si>
+    <t>Age group of respondents (e.g., "10-19")</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA10A4EA-A525-E944-8D72-CB2BE2F27B9F}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,13 +1034,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1072,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1083,10 +1059,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1094,10 +1070,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,10 +1081,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1116,10 +1092,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1127,10 +1103,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1138,10 +1114,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1149,10 +1125,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1160,10 +1136,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1171,10 +1147,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1182,10 +1158,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1193,10 +1169,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1204,10 +1180,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1215,10 +1191,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1226,10 +1202,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1237,10 +1213,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1248,10 +1224,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1259,10 +1235,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1270,10 +1246,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,10 +1257,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1292,10 +1268,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1303,10 +1279,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +1290,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +1301,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,10 +1312,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,10 +1323,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1358,10 +1334,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,10 +1345,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,10 +1356,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,10 +1367,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,10 +1378,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,10 +1389,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,10 +1400,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,10 +1411,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1446,10 +1422,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1457,10 +1433,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,10 +1444,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1479,10 +1455,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1490,10 +1466,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1501,10 +1477,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1512,10 +1488,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,10 +1499,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1534,10 +1510,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,10 +1521,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,10 +1532,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,10 +1543,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1578,10 +1554,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1591,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1C608A-3A12-6A4E-B5EF-A03A944D5F26}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,13 +1581,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1619,10 +1595,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1630,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1641,10 +1617,10 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1652,10 +1628,10 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1663,10 +1639,10 @@
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1674,10 +1650,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,10 +1661,10 @@
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1696,10 +1672,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1707,10 +1683,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1718,318 +1694,252 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
         <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" t="s">
-        <v>180</v>
-      </c>
-      <c r="C35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" t="s">
-        <v>202</v>
-      </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" t="s">
-        <v>203</v>
-      </c>
-      <c r="C38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2041,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B676526F-B79A-FC4F-B63F-B998E01063BD}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2052,13 +1962,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2066,10 +1976,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2077,109 +1987,109 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2187,10 +2097,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2198,10 +2108,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,10 +2119,10 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2220,10 +2130,10 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2231,10 +2141,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2242,10 +2152,10 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2253,10 +2163,10 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,10 +2174,10 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2275,10 +2185,10 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,32 +2196,32 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,10 +2229,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,10 +2240,10 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2341,10 +2251,10 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2352,10 +2262,10 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2363,10 +2273,10 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2374,142 +2284,142 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2517,10 +2427,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2528,10 +2438,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2539,10 +2449,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2550,10 +2460,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2561,10 +2471,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2576,21 +2486,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EB01E8-31A6-B647-9BA6-C61F8F9A982B}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="3" width="49.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2598,10 +2512,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2609,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2620,10 +2534,10 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2631,10 +2545,10 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2642,10 +2556,10 @@
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2653,10 +2567,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2664,21 +2578,21 @@
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2686,10 +2600,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2697,296 +2611,296 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>